<commit_message>
Manual update of coordinates for Monday trivia
Confirm that coordinates are precise for all the Monday trivia events and update for the imprecise coordinates.
</commit_message>
<xml_diff>
--- a/data/final_trivia_list.xlsx
+++ b/data/final_trivia_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KushagraMahaseth/Desktop/cbus_trivia_map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAE8437-9103-8247-B353-DC62393AD89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB24A18D-1DC6-4340-8EF6-A350380660EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36420" yWindow="0" windowWidth="28800" windowHeight="28780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57260" yWindow="0" windowWidth="13700" windowHeight="28780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1266,7 +1266,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1323,7 +1323,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1629,7 +1629,7 @@
   <dimension ref="A1:I183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1773,10 +1773,10 @@
         <v>13</v>
       </c>
       <c r="H5">
-        <v>39.985785700000001</v>
+        <v>39.985329</v>
       </c>
       <c r="I5" s="2">
-        <v>-82.999961600000006</v>
+        <v>-82.999964899999995</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1825,10 +1825,10 @@
         <v>13</v>
       </c>
       <c r="H7">
-        <v>40.148654000000001</v>
+        <v>40.149920999999999</v>
       </c>
       <c r="I7" s="2">
-        <v>-82.978968800000004</v>
+        <v>-82.979111000000003</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1851,10 +1851,10 @@
         <v>13</v>
       </c>
       <c r="H8">
-        <v>40.080894600000001</v>
+        <v>40.082180000000001</v>
       </c>
       <c r="I8">
-        <v>-82.810828999999998</v>
+        <v>-82.810730000000007</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Manual coordinate updates for Tuesday events
</commit_message>
<xml_diff>
--- a/data/final_trivia_list.xlsx
+++ b/data/final_trivia_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KushagraMahaseth/Desktop/cbus_trivia_map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB24A18D-1DC6-4340-8EF6-A350380660EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBDD5C0-E936-914F-8DDC-A867CDBECD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57260" yWindow="0" windowWidth="13700" windowHeight="28780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="26600" windowHeight="28780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1265,8 +1265,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1318,12 +1319,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1628,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2022,10 +2024,10 @@
         <v>52</v>
       </c>
       <c r="H14">
-        <v>39.996240999999998</v>
+        <v>39.997681</v>
       </c>
       <c r="I14">
-        <v>-82.843470699999997</v>
+        <v>-82.842781000000002</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2080,10 +2082,10 @@
         <v>52</v>
       </c>
       <c r="H16">
-        <v>40.091343199999997</v>
+        <v>40.084685</v>
       </c>
       <c r="I16">
-        <v>-82.893214400000005</v>
+        <v>-82.894772000000003</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -2108,11 +2110,11 @@
       <c r="G17" t="s">
         <v>52</v>
       </c>
-      <c r="H17">
-        <v>40.107888799999998</v>
+      <c r="H17" s="3">
+        <v>40.107300000000002</v>
       </c>
       <c r="I17">
-        <v>-83.271337900000006</v>
+        <v>-83.268592999999996</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -2138,10 +2140,10 @@
         <v>52</v>
       </c>
       <c r="H18">
-        <v>40.585690700000001</v>
+        <v>40.092458999999998</v>
       </c>
       <c r="I18">
-        <v>-82.422275799999994</v>
+        <v>-83.017568999999995</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -2225,10 +2227,10 @@
         <v>52</v>
       </c>
       <c r="H21">
-        <v>40.094974399999998</v>
+        <v>40.106014000000002</v>
       </c>
       <c r="I21">
-        <v>-82.998063900000005</v>
+        <v>-82.997749999999996</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -2341,10 +2343,10 @@
         <v>52</v>
       </c>
       <c r="H25">
-        <v>40.287680999999999</v>
+        <v>40.135131999999999</v>
       </c>
       <c r="I25">
-        <v>-82.283842000000007</v>
+        <v>-82.989188999999996</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Verify and update coordinates for Tuesday events
Double check the coordinates of all the bars with trivia night on Tuesday and adjust the coordinates which imprecise
</commit_message>
<xml_diff>
--- a/data/final_trivia_list.xlsx
+++ b/data/final_trivia_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KushagraMahaseth/Desktop/cbus_trivia_map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBDD5C0-E936-914F-8DDC-A867CDBECD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9A762C-7A50-434D-BAA7-F47562C7AD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="26600" windowHeight="28780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="21520" windowHeight="28780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1630,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2430,10 +2430,10 @@
         <v>52</v>
       </c>
       <c r="H28">
-        <v>40.066765400000001</v>
+        <v>40.066738000000001</v>
       </c>
       <c r="I28">
-        <v>-82.519197700000007</v>
+        <v>-82.519231000000005</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -2459,10 +2459,10 @@
         <v>52</v>
       </c>
       <c r="H29">
-        <v>40.151955600000001</v>
-      </c>
-      <c r="I29">
-        <v>-82.683034899999996</v>
+        <v>40.152678000000002</v>
+      </c>
+      <c r="I29" s="2">
+        <v>-82.684000999999995</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -2514,10 +2514,10 @@
         <v>52</v>
       </c>
       <c r="H31">
-        <v>40.050178000000002</v>
+        <v>40.061974999999997</v>
       </c>
       <c r="I31">
-        <v>-82.554872000000003</v>
+        <v>-83.173540000000003</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2540,10 +2540,10 @@
         <v>52</v>
       </c>
       <c r="H32">
-        <v>40.057545900000001</v>
+        <v>40.060968000000003</v>
       </c>
       <c r="I32">
-        <v>-82.849220399999993</v>
+        <v>-82.848586999999995</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -2592,10 +2592,10 @@
         <v>52</v>
       </c>
       <c r="H34">
-        <v>40.102353299999997</v>
+        <v>40.104647999999997</v>
       </c>
       <c r="I34">
-        <v>-83.109618600000005</v>
+        <v>-83.109679</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -2618,10 +2618,10 @@
         <v>52</v>
       </c>
       <c r="H35">
-        <v>40.133350999999998</v>
+        <v>40.134905000000003</v>
       </c>
       <c r="I35">
-        <v>-83.070931000000002</v>
+        <v>-83.071707000000004</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -2670,10 +2670,10 @@
         <v>52</v>
       </c>
       <c r="H37">
-        <v>40.017609</v>
+        <v>40.001173999999999</v>
       </c>
       <c r="I37">
-        <v>-83.158304799999996</v>
+        <v>-83.155935999999997</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -2699,10 +2699,10 @@
         <v>52</v>
       </c>
       <c r="H38">
-        <v>40.033000600000001</v>
+        <v>40.029060999999999</v>
       </c>
       <c r="I38">
-        <v>-83.116753000000003</v>
+        <v>-83.119546999999997</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -2725,10 +2725,10 @@
         <v>52</v>
       </c>
       <c r="H39">
-        <v>40.133271000000001</v>
-      </c>
-      <c r="I39">
-        <v>-82.929938000000007</v>
+        <v>40.091946</v>
+      </c>
+      <c r="I39" s="2">
+        <v>-82.851022</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -2777,10 +2777,10 @@
         <v>52</v>
       </c>
       <c r="H41">
-        <v>40.080894600000001</v>
+        <v>40.082180000000001</v>
       </c>
       <c r="I41">
-        <v>-82.807458199999999</v>
+        <v>-82.810730000000007</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -2803,10 +2803,10 @@
         <v>52</v>
       </c>
       <c r="H42">
-        <v>39.957345400000001</v>
+        <v>39.957180000000001</v>
       </c>
       <c r="I42">
-        <v>-83.012040499999998</v>
+        <v>-83.012352000000007</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -2855,10 +2855,10 @@
         <v>52</v>
       </c>
       <c r="H44">
-        <v>40.0888785</v>
+        <v>40.089894000000001</v>
       </c>
       <c r="I44">
-        <v>-83.023249699999994</v>
+        <v>-83.050516999999999</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -2881,10 +2881,10 @@
         <v>52</v>
       </c>
       <c r="H45">
-        <v>40.163393200000002</v>
+        <v>40.163246000000001</v>
       </c>
       <c r="I45">
-        <v>-83.074519499999994</v>
+        <v>-83.073654000000005</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -2907,10 +2907,10 @@
         <v>52</v>
       </c>
       <c r="H46">
-        <v>40.057901000000001</v>
+        <v>40.107474000000003</v>
       </c>
       <c r="I46">
-        <v>-83.307322999999997</v>
+        <v>-83.191834999999998</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -3118,10 +3118,10 @@
         <v>52</v>
       </c>
       <c r="H54">
-        <v>40.034937300000003</v>
-      </c>
-      <c r="I54">
-        <v>-83.160943500000002</v>
+        <v>40.034574999999997</v>
+      </c>
+      <c r="I54" s="2">
+        <v>-83.160045999999994</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -3201,11 +3201,11 @@
       <c r="G57" t="s">
         <v>52</v>
       </c>
-      <c r="H57">
-        <v>40.157209799999997</v>
+      <c r="H57" s="3">
+        <v>40.156796</v>
       </c>
       <c r="I57">
-        <v>-83.088352999999998</v>
+        <v>-83.087918999999999</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -3228,10 +3228,10 @@
         <v>52</v>
       </c>
       <c r="H58">
-        <v>39.997445599999999</v>
+        <v>39.995246000000002</v>
       </c>
       <c r="I58">
-        <v>-83.074344199999999</v>
+        <v>-83.072159999999997</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -3253,11 +3253,11 @@
       <c r="G59" t="s">
         <v>52</v>
       </c>
-      <c r="H59">
-        <v>39.949621800000003</v>
+      <c r="H59" s="3">
+        <v>39.949798999999999</v>
       </c>
       <c r="I59">
-        <v>-82.982655199999996</v>
+        <v>-82.982680999999999</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -3312,10 +3312,10 @@
         <v>52</v>
       </c>
       <c r="H61">
-        <v>39.924048999999997</v>
+        <v>39.923730999999997</v>
       </c>
       <c r="I61">
-        <v>-82.782620199999997</v>
+        <v>-82.783563000000001</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -3338,10 +3338,10 @@
         <v>52</v>
       </c>
       <c r="H62">
-        <v>40.054847500000001</v>
+        <v>40.054747999999996</v>
       </c>
       <c r="I62">
-        <v>-82.913042799999999</v>
+        <v>-82.912868000000003</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -3416,10 +3416,10 @@
         <v>52</v>
       </c>
       <c r="H65">
-        <v>40.1092206</v>
+        <v>40.109527999999997</v>
       </c>
       <c r="I65">
-        <v>-83.000199199999997</v>
+        <v>-82.999432999999996</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -3497,10 +3497,10 @@
         <v>52</v>
       </c>
       <c r="H68">
-        <v>40.306662600000003</v>
+        <v>40.306669999999997</v>
       </c>
       <c r="I68">
-        <v>-83.090237000000002</v>
+        <v>-83.089072000000002</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Verify and update coordinates of Fri-Sun trivias
</commit_message>
<xml_diff>
--- a/data/final_trivia_list.xlsx
+++ b/data/final_trivia_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KushagraMahaseth/Desktop/cbus_trivia_map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9A762C-7A50-434D-BAA7-F47562C7AD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA189048-7AB8-704B-925A-72AC1A400F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="0" windowWidth="21520" windowHeight="28780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1630,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="H183" sqref="H183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6339,10 +6339,10 @@
         <v>392</v>
       </c>
       <c r="H172">
-        <v>39.957345400000001</v>
+        <v>39.957180000000001</v>
       </c>
       <c r="I172">
-        <v>-83.012040499999998</v>
+        <v>-83.012352000000007</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
@@ -6368,10 +6368,10 @@
         <v>392</v>
       </c>
       <c r="H173">
-        <v>40.295212999999997</v>
+        <v>40.296548000000001</v>
       </c>
       <c r="I173">
-        <v>-83.448864</v>
+        <v>-83.449252000000001</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
@@ -6426,10 +6426,10 @@
         <v>401</v>
       </c>
       <c r="H175">
-        <v>40.298800999999997</v>
+        <v>40.298985999999999</v>
       </c>
       <c r="I175">
-        <v>-83.067770999999993</v>
+        <v>-83.067916999999994</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
@@ -6455,10 +6455,10 @@
         <v>401</v>
       </c>
       <c r="H176">
-        <v>40.023539</v>
+        <v>40.020870000000002</v>
       </c>
       <c r="I176">
-        <v>-82.866252700000004</v>
+        <v>-82.866675999999998</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
@@ -6481,10 +6481,10 @@
         <v>401</v>
       </c>
       <c r="H177">
-        <v>40.110565800000003</v>
+        <v>40.111477999999998</v>
       </c>
       <c r="I177">
-        <v>-82.944723499999995</v>
+        <v>-82.945682000000005</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
@@ -6538,11 +6538,11 @@
       <c r="G179" t="s">
         <v>402</v>
       </c>
-      <c r="H179">
-        <v>40.000195099999999</v>
+      <c r="H179" s="3">
+        <v>40.000301</v>
       </c>
       <c r="I179">
-        <v>-82.998603500000002</v>
+        <v>-82.998322000000002</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
@@ -6591,10 +6591,10 @@
         <v>402</v>
       </c>
       <c r="H181">
-        <v>39.981001900000003</v>
+        <v>39.981107999999999</v>
       </c>
       <c r="I181">
-        <v>-82.998547900000005</v>
+        <v>-82.998925</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
@@ -6620,10 +6620,10 @@
         <v>402</v>
       </c>
       <c r="H182">
-        <v>40.022365000000001</v>
+        <v>40.022682000000003</v>
       </c>
       <c r="I182">
-        <v>-83.013552000000004</v>
+        <v>-83.014105000000001</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Verify and update coordinates of Thursday's events
</commit_message>
<xml_diff>
--- a/data/final_trivia_list.xlsx
+++ b/data/final_trivia_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KushagraMahaseth/Desktop/cbus_trivia_map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA189048-7AB8-704B-925A-72AC1A400F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D7A924-3CA9-B843-995E-2E6135951C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="21520" windowHeight="28780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28880" yWindow="0" windowWidth="21520" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1269,7 +1269,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1282,6 +1282,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1319,13 +1326,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1630,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="H183" sqref="H183"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="K144" sqref="K144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5273,11 +5282,11 @@
       <c r="G133" t="s">
         <v>328</v>
       </c>
-      <c r="H133">
-        <v>40.133271000000001</v>
-      </c>
-      <c r="I133">
-        <v>-82.929938000000007</v>
+      <c r="H133" s="4">
+        <v>40.091949999999997</v>
+      </c>
+      <c r="I133" s="5">
+        <v>-82.850999999999999</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
@@ -5363,7 +5372,7 @@
       <c r="H136">
         <v>39.955039499999998</v>
       </c>
-      <c r="I136">
+      <c r="I136" s="2">
         <v>-82.998959299999996</v>
       </c>
     </row>
@@ -5390,10 +5399,10 @@
         <v>328</v>
       </c>
       <c r="H137">
-        <v>40.154178999999999</v>
+        <v>40.154406999999999</v>
       </c>
       <c r="I137">
-        <v>-82.924636000000007</v>
+        <v>-82.923344999999998</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
@@ -5505,11 +5514,11 @@
       <c r="G141" t="s">
         <v>328</v>
       </c>
-      <c r="H141">
-        <v>40.155147999999997</v>
+      <c r="H141" s="3">
+        <v>40.155399000000003</v>
       </c>
       <c r="I141">
-        <v>-83.012860000000003</v>
+        <v>-83.012512000000001</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -5648,10 +5657,10 @@
         <v>328</v>
       </c>
       <c r="H146">
-        <v>39.973030999999999</v>
+        <v>39.972866000000003</v>
       </c>
       <c r="I146">
-        <v>-82.899229000000005</v>
+        <v>-82.899394000000001</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
@@ -5674,10 +5683,10 @@
         <v>328</v>
       </c>
       <c r="H147">
-        <v>40.152441000000003</v>
+        <v>40.151738999999999</v>
       </c>
       <c r="I147">
-        <v>-82.996729999999999</v>
+        <v>-82.995913999999999</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -5700,10 +5709,10 @@
         <v>328</v>
       </c>
       <c r="H148">
-        <v>40.017609</v>
+        <v>40.001175000000003</v>
       </c>
       <c r="I148">
-        <v>-83.158304799999996</v>
+        <v>-83.155936999999994</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -5726,10 +5735,10 @@
         <v>328</v>
       </c>
       <c r="H149">
-        <v>40.014480800000001</v>
+        <v>40.014431000000002</v>
       </c>
       <c r="I149">
-        <v>-83.013632599999994</v>
+        <v>-83.014221000000006</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
@@ -5751,11 +5760,11 @@
       <c r="G150" t="s">
         <v>328</v>
       </c>
-      <c r="H150">
-        <v>40.237314900000001</v>
+      <c r="H150" s="3">
+        <v>40.237394999999999</v>
       </c>
       <c r="I150">
-        <v>-83.362372300000004</v>
+        <v>-83.362556999999995</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
@@ -5830,10 +5839,10 @@
         <v>328</v>
       </c>
       <c r="H153">
-        <v>39.881501999999998</v>
+        <v>39.881630000000001</v>
       </c>
       <c r="I153">
-        <v>-83.094323000000003</v>
+        <v>-83.094322000000005</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
@@ -5882,10 +5891,10 @@
         <v>328</v>
       </c>
       <c r="H155">
-        <v>39.759580999999997</v>
-      </c>
-      <c r="I155">
-        <v>-82.666860999999997</v>
+        <v>39.760269000000001</v>
+      </c>
+      <c r="I155" s="2">
+        <v>-82.666267000000005</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
@@ -5908,10 +5917,10 @@
         <v>328</v>
       </c>
       <c r="H156">
-        <v>40.051666500000003</v>
+        <v>40.051938</v>
       </c>
       <c r="I156">
-        <v>-82.920055099999999</v>
+        <v>-82.920542999999995</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -5934,10 +5943,10 @@
         <v>328</v>
       </c>
       <c r="H157">
-        <v>40.118285</v>
-      </c>
-      <c r="I157">
-        <v>-82.986973599999999</v>
+        <v>40.117525999999998</v>
+      </c>
+      <c r="I157" s="2">
+        <v>-82.986984000000007</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -5960,10 +5969,10 @@
         <v>328</v>
       </c>
       <c r="H158">
-        <v>40.1486065</v>
+        <v>40.149245999999998</v>
       </c>
       <c r="I158">
-        <v>-83.090912200000005</v>
+        <v>-83.091482999999997</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -6128,10 +6137,10 @@
         <v>328</v>
       </c>
       <c r="H164">
-        <v>39.880029999999998</v>
+        <v>39.880431999999999</v>
       </c>
       <c r="I164">
-        <v>-83.069728499999997</v>
+        <v>-83.070642000000007</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
@@ -6183,10 +6192,10 @@
         <v>328</v>
       </c>
       <c r="H166">
-        <v>40.061228</v>
+        <v>40.061892999999998</v>
       </c>
       <c r="I166">
-        <v>-83.075224000000006</v>
+        <v>-83.075406999999998</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
@@ -6235,10 +6244,10 @@
         <v>328</v>
       </c>
       <c r="H168">
-        <v>40.163406899999998</v>
+        <v>40.163572000000002</v>
       </c>
       <c r="I168">
-        <v>-83.074968699999999</v>
+        <v>-83.074144000000004</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.2">
@@ -6261,10 +6270,10 @@
         <v>328</v>
       </c>
       <c r="H169">
-        <v>39.885176299999998</v>
+        <v>39.885311000000002</v>
       </c>
       <c r="I169">
-        <v>-82.755675400000001</v>
+        <v>-82.754822000000004</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Verify, update, and add Wed trivia events
Add Nocterra in addition to manually fixing coordinates to the Wednesday trivia events
</commit_message>
<xml_diff>
--- a/data/final_trivia_list.xlsx
+++ b/data/final_trivia_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KushagraMahaseth/Desktop/cbus_trivia_map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D7A924-3CA9-B843-995E-2E6135951C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385099A1-7F87-E843-8D5A-7FC56C5EA22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28880" yWindow="0" windowWidth="21520" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="23060" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="415">
   <si>
     <t>Bar</t>
   </si>
@@ -1259,6 +1259,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 2971 N High St, Columbus, OH 43202 </t>
+  </si>
+  <si>
+    <t>Nocterra Brewing Co</t>
+  </si>
+  <si>
+    <t>41 Depot St, Powell, OH 43065</t>
   </si>
 </sst>
 </file>
@@ -1637,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I183"/>
+  <dimension ref="A1:I184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="K144" sqref="K144"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="Q148" sqref="Q148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3619,10 +3625,10 @@
         <v>194</v>
       </c>
       <c r="H72">
-        <v>40.0645332</v>
+        <v>40.065545999999998</v>
       </c>
       <c r="I72">
-        <v>-82.861620299999998</v>
+        <v>-82.861662999999993</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -3735,10 +3741,10 @@
         <v>194</v>
       </c>
       <c r="H76">
-        <v>40.049171100000002</v>
+        <v>40.049261999999999</v>
       </c>
       <c r="I76">
-        <v>-82.916895600000004</v>
+        <v>-82.917013999999995</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -3764,10 +3770,10 @@
         <v>194</v>
       </c>
       <c r="H77">
-        <v>40.152661999999999</v>
+        <v>40.152481000000002</v>
       </c>
       <c r="I77">
-        <v>-82.996663999999996</v>
+        <v>-82.995879000000002</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -3822,10 +3828,10 @@
         <v>194</v>
       </c>
       <c r="H79">
-        <v>39.9977272</v>
+        <v>39.997658999999999</v>
       </c>
       <c r="I79">
-        <v>-83.006279199999994</v>
+        <v>-83.006963999999996</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -3909,10 +3915,10 @@
         <v>194</v>
       </c>
       <c r="H82">
-        <v>40.113782200000003</v>
+        <v>40.114787999999997</v>
       </c>
       <c r="I82">
-        <v>-83.012888099999998</v>
+        <v>-83.011163999999994</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -3966,7 +3972,7 @@
       <c r="G84" t="s">
         <v>194</v>
       </c>
-      <c r="H84">
+      <c r="H84" s="3">
         <v>39.962494999999997</v>
       </c>
       <c r="I84">
@@ -4024,11 +4030,11 @@
       <c r="G86" t="s">
         <v>194</v>
       </c>
-      <c r="H86">
-        <v>40.132798399999999</v>
+      <c r="H86" s="3">
+        <v>40.132401999999999</v>
       </c>
       <c r="I86">
-        <v>-82.918042600000007</v>
+        <v>-82.887263000000004</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
@@ -4112,10 +4118,10 @@
         <v>194</v>
       </c>
       <c r="H89">
-        <v>40.0638583</v>
+        <v>40.065072999999998</v>
       </c>
       <c r="I89">
-        <v>-83.058728599999995</v>
+        <v>-83.058170000000004</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
@@ -4189,7 +4195,7 @@
       <c r="G92" t="s">
         <v>194</v>
       </c>
-      <c r="H92">
+      <c r="H92" s="3">
         <v>40.025897000000001</v>
       </c>
       <c r="I92">
@@ -4297,10 +4303,10 @@
         <v>194</v>
       </c>
       <c r="H96">
-        <v>40.133350999999998</v>
+        <v>40.134905000000003</v>
       </c>
       <c r="I96">
-        <v>-83.070931000000002</v>
+        <v>-83.071707000000004</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
@@ -4323,10 +4329,10 @@
         <v>194</v>
       </c>
       <c r="H97">
-        <v>40.017609</v>
+        <v>40.001175000000003</v>
       </c>
       <c r="I97">
-        <v>-83.158304799999996</v>
+        <v>-83.155936999999994</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
@@ -4375,10 +4381,10 @@
         <v>194</v>
       </c>
       <c r="H99">
-        <v>40.055719099999997</v>
+        <v>40.063189000000001</v>
       </c>
       <c r="I99">
-        <v>-83.126540300000002</v>
+        <v>-83.128542999999993</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
@@ -4401,10 +4407,10 @@
         <v>194</v>
       </c>
       <c r="H100">
-        <v>40.001906900000002</v>
+        <v>40.002828999999998</v>
       </c>
       <c r="I100">
-        <v>-83.184967499999999</v>
+        <v>-83.150968000000006</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
@@ -4453,10 +4459,10 @@
         <v>194</v>
       </c>
       <c r="H102">
-        <v>40.110565800000003</v>
+        <v>40.111477000000001</v>
       </c>
       <c r="I102">
-        <v>-82.944723499999995</v>
+        <v>-82.945678999999998</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
@@ -4505,10 +4511,10 @@
         <v>194</v>
       </c>
       <c r="H104">
-        <v>40.236240000000002</v>
+        <v>40.235933000000003</v>
       </c>
       <c r="I104">
-        <v>-83.367014999999995</v>
+        <v>-83.367222999999996</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
@@ -4531,10 +4537,10 @@
         <v>194</v>
       </c>
       <c r="H105">
-        <v>39.843274299999997</v>
+        <v>39.843274000000001</v>
       </c>
       <c r="I105">
-        <v>-82.806872900000002</v>
+        <v>-82.807066000000006</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
@@ -4583,10 +4589,10 @@
         <v>194</v>
       </c>
       <c r="H107">
-        <v>40.040259599999999</v>
+        <v>40.039116</v>
       </c>
       <c r="I107">
-        <v>-83.179708199999993</v>
+        <v>-83.180047000000002</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
@@ -4609,10 +4615,10 @@
         <v>194</v>
       </c>
       <c r="H108">
-        <v>40.023668999999998</v>
+        <v>40.023550999999998</v>
       </c>
       <c r="I108">
-        <v>-83.162728999999999</v>
+        <v>-83.162335999999996</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
@@ -4687,10 +4693,10 @@
         <v>194</v>
       </c>
       <c r="H111">
-        <v>40.081641500000003</v>
+        <v>40.079335999999998</v>
       </c>
       <c r="I111">
-        <v>-82.823351799999998</v>
+        <v>-82.849553999999998</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
@@ -4713,10 +4719,10 @@
         <v>194</v>
       </c>
       <c r="H112">
-        <v>40.064095799999997</v>
+        <v>40.063479000000001</v>
       </c>
       <c r="I112">
-        <v>-83.019303600000001</v>
+        <v>-83.019031999999996</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
@@ -4765,10 +4771,10 @@
         <v>194</v>
       </c>
       <c r="H114">
-        <v>39.984211999999999</v>
+        <v>40.166336000000001</v>
       </c>
       <c r="I114">
-        <v>-82.458113999999995</v>
+        <v>-83.186271000000005</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
@@ -4791,10 +4797,10 @@
         <v>194</v>
       </c>
       <c r="H115">
-        <v>40.154691</v>
+        <v>40.154936999999997</v>
       </c>
       <c r="I115">
-        <v>-83.093993999999995</v>
+        <v>-83.094705000000005</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
@@ -4817,10 +4823,10 @@
         <v>194</v>
       </c>
       <c r="H116">
-        <v>40.101963300000001</v>
-      </c>
-      <c r="I116">
-        <v>-82.786050900000006</v>
+        <v>40.101053999999998</v>
+      </c>
+      <c r="I116" s="3">
+        <v>-82.786101000000002</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
@@ -5011,10 +5017,10 @@
         <v>194</v>
       </c>
       <c r="H123">
-        <v>40.057038400000003</v>
+        <v>40.057467000000003</v>
       </c>
       <c r="I123">
-        <v>-83.074652999999998</v>
+        <v>-83.074375000000003</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
@@ -5065,11 +5071,11 @@
       <c r="G125" t="s">
         <v>194</v>
       </c>
-      <c r="H125">
-        <v>40.023539</v>
-      </c>
-      <c r="I125">
-        <v>-82.866252700000004</v>
+      <c r="H125" s="4">
+        <v>40.020870000000002</v>
+      </c>
+      <c r="I125" s="4">
+        <v>-82.866699999999994</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -5095,10 +5101,10 @@
         <v>194</v>
       </c>
       <c r="H126">
-        <v>40.149051900000003</v>
+        <v>40.150357999999997</v>
       </c>
       <c r="I126">
-        <v>-82.922627300000002</v>
+        <v>-82.922230999999996</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
@@ -5121,10 +5127,10 @@
         <v>194</v>
       </c>
       <c r="H127">
-        <v>40.018422000000001</v>
+        <v>40.033768000000002</v>
       </c>
       <c r="I127">
-        <v>-83.135835</v>
+        <v>-83.180301</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
@@ -5147,10 +5153,10 @@
         <v>194</v>
       </c>
       <c r="H128">
-        <v>40.299678999999998</v>
+        <v>40.299641000000001</v>
       </c>
       <c r="I128">
-        <v>-83.067802999999998</v>
+        <v>-83.067993000000001</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -5199,10 +5205,10 @@
         <v>194</v>
       </c>
       <c r="H130">
-        <v>39.984814999999998</v>
+        <v>39.985036999999998</v>
       </c>
       <c r="I130">
-        <v>-83.036181999999997</v>
+        <v>-83.036681999999999</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
@@ -5228,10 +5234,10 @@
         <v>194</v>
       </c>
       <c r="H131">
-        <v>40.0570156</v>
+        <v>40.057949999999998</v>
       </c>
       <c r="I131">
-        <v>-82.455908100000002</v>
+        <v>-82.456159</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
@@ -5254,10 +5260,10 @@
         <v>194</v>
       </c>
       <c r="H132">
-        <v>39.842565499999999</v>
+        <v>39.842376999999999</v>
       </c>
       <c r="I132">
-        <v>-82.805751200000003</v>
+        <v>-82.805880000000002</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
@@ -5265,28 +5271,25 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>120</v>
+        <v>413</v>
       </c>
       <c r="C133" t="s">
-        <v>9</v>
-      </c>
-      <c r="D133" t="s">
-        <v>327</v>
+        <v>172</v>
       </c>
       <c r="E133" t="s">
         <v>11</v>
       </c>
       <c r="F133" t="s">
-        <v>121</v>
+        <v>414</v>
       </c>
       <c r="G133" t="s">
-        <v>328</v>
-      </c>
-      <c r="H133" s="4">
-        <v>40.091949999999997</v>
-      </c>
-      <c r="I133" s="5">
-        <v>-82.850999999999999</v>
+        <v>194</v>
+      </c>
+      <c r="H133">
+        <v>40.159644999999998</v>
+      </c>
+      <c r="I133">
+        <v>-83.078484000000003</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
@@ -5294,28 +5297,28 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>261</v>
+        <v>120</v>
       </c>
       <c r="C134" t="s">
         <v>9</v>
       </c>
       <c r="D134" t="s">
-        <v>69</v>
+        <v>327</v>
       </c>
       <c r="E134" t="s">
         <v>11</v>
       </c>
       <c r="F134" t="s">
-        <v>262</v>
+        <v>121</v>
       </c>
       <c r="G134" t="s">
         <v>328</v>
       </c>
-      <c r="H134">
-        <v>40.123615200000003</v>
-      </c>
-      <c r="I134">
-        <v>-82.981080700000007</v>
+      <c r="H134" s="4">
+        <v>40.091949999999997</v>
+      </c>
+      <c r="I134" s="5">
+        <v>-82.850999999999999</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
@@ -5323,28 +5326,28 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>56</v>
+        <v>261</v>
       </c>
       <c r="C135" t="s">
         <v>9</v>
       </c>
       <c r="D135" t="s">
-        <v>329</v>
+        <v>69</v>
       </c>
       <c r="E135" t="s">
         <v>11</v>
       </c>
       <c r="F135" t="s">
-        <v>58</v>
+        <v>262</v>
       </c>
       <c r="G135" t="s">
         <v>328</v>
       </c>
       <c r="H135">
-        <v>39.987723099999997</v>
+        <v>40.123615200000003</v>
       </c>
       <c r="I135">
-        <v>-83.030377700000003</v>
+        <v>-82.981080700000007</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
@@ -5352,28 +5355,28 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>330</v>
+        <v>56</v>
       </c>
       <c r="C136" t="s">
         <v>9</v>
       </c>
       <c r="D136" t="s">
-        <v>10</v>
+        <v>329</v>
       </c>
       <c r="E136" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F136" t="s">
-        <v>331</v>
+        <v>58</v>
       </c>
       <c r="G136" t="s">
         <v>328</v>
       </c>
       <c r="H136">
-        <v>39.955039499999998</v>
-      </c>
-      <c r="I136" s="2">
-        <v>-82.998959299999996</v>
+        <v>39.987723099999997</v>
+      </c>
+      <c r="I136">
+        <v>-83.030377700000003</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
@@ -5381,28 +5384,28 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C137" t="s">
         <v>9</v>
       </c>
       <c r="D137" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="E137" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="F137" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G137" t="s">
         <v>328</v>
       </c>
       <c r="H137">
-        <v>40.154406999999999</v>
-      </c>
-      <c r="I137">
-        <v>-82.923344999999998</v>
+        <v>39.955039499999998</v>
+      </c>
+      <c r="I137" s="2">
+        <v>-82.998959299999996</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
@@ -5410,28 +5413,28 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>199</v>
+        <v>332</v>
       </c>
       <c r="C138" t="s">
         <v>9</v>
       </c>
       <c r="D138" t="s">
-        <v>334</v>
+        <v>54</v>
       </c>
       <c r="E138" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F138" t="s">
-        <v>201</v>
+        <v>333</v>
       </c>
       <c r="G138" t="s">
         <v>328</v>
       </c>
       <c r="H138">
-        <v>39.956913399999998</v>
+        <v>40.154406999999999</v>
       </c>
       <c r="I138">
-        <v>-82.9934978</v>
+        <v>-82.923344999999998</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
@@ -5439,28 +5442,28 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>335</v>
+        <v>199</v>
       </c>
       <c r="C139" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D139" t="s">
-        <v>227</v>
+        <v>334</v>
       </c>
       <c r="E139" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F139" t="s">
-        <v>336</v>
+        <v>201</v>
       </c>
       <c r="G139" t="s">
         <v>328</v>
       </c>
       <c r="H139">
-        <v>40.050076099999998</v>
+        <v>39.956913399999998</v>
       </c>
       <c r="I139">
-        <v>-82.915329099999994</v>
+        <v>-82.9934978</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
@@ -5468,28 +5471,28 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C140" t="s">
         <v>15</v>
       </c>
       <c r="D140" t="s">
-        <v>167</v>
+        <v>227</v>
       </c>
       <c r="E140" t="s">
         <v>11</v>
       </c>
       <c r="F140" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G140" t="s">
         <v>328</v>
       </c>
       <c r="H140">
-        <v>39.981029700000001</v>
+        <v>40.050076099999998</v>
       </c>
       <c r="I140">
-        <v>-83.0040707</v>
+        <v>-82.915329099999994</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
@@ -5497,28 +5500,28 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C141" t="s">
         <v>15</v>
       </c>
       <c r="D141" t="s">
-        <v>230</v>
+        <v>167</v>
       </c>
       <c r="E141" t="s">
         <v>11</v>
       </c>
       <c r="F141" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G141" t="s">
         <v>328</v>
       </c>
-      <c r="H141" s="3">
-        <v>40.155399000000003</v>
+      <c r="H141">
+        <v>39.981029700000001</v>
       </c>
       <c r="I141">
-        <v>-83.012512000000001</v>
+        <v>-83.0040707</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -5526,28 +5529,28 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C142" t="s">
         <v>15</v>
       </c>
       <c r="D142" t="s">
-        <v>342</v>
+        <v>230</v>
       </c>
       <c r="E142" t="s">
         <v>11</v>
       </c>
       <c r="F142" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G142" t="s">
         <v>328</v>
       </c>
-      <c r="H142">
-        <v>39.972353400000003</v>
+      <c r="H142" s="3">
+        <v>40.155399000000003</v>
       </c>
       <c r="I142">
-        <v>-83.004915100000005</v>
+        <v>-83.012512000000001</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -5555,28 +5558,28 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C143" t="s">
         <v>15</v>
       </c>
       <c r="D143" t="s">
-        <v>16</v>
+        <v>342</v>
       </c>
       <c r="E143" t="s">
         <v>11</v>
       </c>
       <c r="F143" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G143" t="s">
         <v>328</v>
       </c>
       <c r="H143">
-        <v>39.903026099999998</v>
+        <v>39.972353400000003</v>
       </c>
       <c r="I143">
-        <v>-82.776906600000004</v>
+        <v>-83.004915100000005</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
@@ -5584,28 +5587,28 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>296</v>
+        <v>344</v>
       </c>
       <c r="C144" t="s">
         <v>15</v>
       </c>
       <c r="D144" t="s">
-        <v>346</v>
+        <v>16</v>
       </c>
       <c r="E144" t="s">
         <v>11</v>
       </c>
       <c r="F144" t="s">
-        <v>298</v>
+        <v>345</v>
       </c>
       <c r="G144" t="s">
         <v>328</v>
       </c>
       <c r="H144">
-        <v>39.965665999999999</v>
+        <v>39.903026099999998</v>
       </c>
       <c r="I144">
-        <v>-82.995581000000001</v>
+        <v>-82.776906600000004</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
@@ -5613,28 +5616,28 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>347</v>
+        <v>296</v>
       </c>
       <c r="C145" t="s">
         <v>15</v>
       </c>
       <c r="D145" t="s">
-        <v>88</v>
+        <v>346</v>
       </c>
       <c r="E145" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F145" t="s">
-        <v>348</v>
+        <v>298</v>
       </c>
       <c r="G145" t="s">
         <v>328</v>
       </c>
       <c r="H145">
-        <v>39.984074200000002</v>
+        <v>39.965665999999999</v>
       </c>
       <c r="I145">
-        <v>-83.015304999999998</v>
+        <v>-82.995581000000001</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -5642,25 +5645,28 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C146" t="s">
-        <v>111</v>
+        <v>15</v>
+      </c>
+      <c r="D146" t="s">
+        <v>88</v>
       </c>
       <c r="E146" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="F146" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G146" t="s">
         <v>328</v>
       </c>
       <c r="H146">
-        <v>39.972866000000003</v>
+        <v>39.984074200000002</v>
       </c>
       <c r="I146">
-        <v>-82.899394000000001</v>
+        <v>-83.015304999999998</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
@@ -5668,25 +5674,25 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C147" t="s">
         <v>111</v>
       </c>
       <c r="E147" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="F147" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G147" t="s">
         <v>328</v>
       </c>
       <c r="H147">
-        <v>40.151738999999999</v>
+        <v>39.972866000000003</v>
       </c>
       <c r="I147">
-        <v>-82.995913999999999</v>
+        <v>-82.899394000000001</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -5694,7 +5700,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>115</v>
+        <v>351</v>
       </c>
       <c r="C148" t="s">
         <v>111</v>
@@ -5703,16 +5709,16 @@
         <v>17</v>
       </c>
       <c r="F148" t="s">
-        <v>116</v>
+        <v>352</v>
       </c>
       <c r="G148" t="s">
         <v>328</v>
       </c>
       <c r="H148">
-        <v>40.001175000000003</v>
+        <v>40.151738999999999</v>
       </c>
       <c r="I148">
-        <v>-83.155936999999994</v>
+        <v>-82.995913999999999</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -5720,25 +5726,25 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>353</v>
+        <v>115</v>
       </c>
       <c r="C149" t="s">
         <v>111</v>
       </c>
       <c r="E149" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F149" t="s">
-        <v>354</v>
+        <v>116</v>
       </c>
       <c r="G149" t="s">
         <v>328</v>
       </c>
       <c r="H149">
-        <v>40.014431000000002</v>
+        <v>40.001175000000003</v>
       </c>
       <c r="I149">
-        <v>-83.014221000000006</v>
+        <v>-83.155936999999994</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
@@ -5746,25 +5752,25 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C150" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E150" t="s">
         <v>11</v>
       </c>
       <c r="F150" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G150" t="s">
         <v>328</v>
       </c>
-      <c r="H150" s="3">
-        <v>40.237394999999999</v>
+      <c r="H150">
+        <v>40.014431000000002</v>
       </c>
       <c r="I150">
-        <v>-83.362556999999995</v>
+        <v>-83.014221000000006</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
@@ -5772,25 +5778,25 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C151" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E151" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F151" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G151" t="s">
         <v>328</v>
       </c>
-      <c r="H151">
-        <v>40.133930999999997</v>
+      <c r="H151" s="3">
+        <v>40.237394999999999</v>
       </c>
       <c r="I151">
-        <v>-83.013186000000005</v>
+        <v>-83.362556999999995</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
@@ -5798,7 +5804,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C152" t="s">
         <v>125</v>
@@ -5807,16 +5813,16 @@
         <v>41</v>
       </c>
       <c r="F152" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G152" t="s">
         <v>328</v>
       </c>
       <c r="H152">
-        <v>40.069232700000001</v>
+        <v>40.133930999999997</v>
       </c>
       <c r="I152">
-        <v>-83.019247899999996</v>
+        <v>-83.013186000000005</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
@@ -5824,25 +5830,25 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C153" t="s">
         <v>125</v>
       </c>
       <c r="E153" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="F153" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G153" t="s">
         <v>328</v>
       </c>
       <c r="H153">
-        <v>39.881630000000001</v>
+        <v>40.069232700000001</v>
       </c>
       <c r="I153">
-        <v>-83.094322000000005</v>
+        <v>-83.019247899999996</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
@@ -5850,7 +5856,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>269</v>
+        <v>361</v>
       </c>
       <c r="C154" t="s">
         <v>125</v>
@@ -5859,16 +5865,16 @@
         <v>11</v>
       </c>
       <c r="F154" t="s">
-        <v>270</v>
+        <v>362</v>
       </c>
       <c r="G154" t="s">
         <v>328</v>
       </c>
       <c r="H154">
-        <v>39.843274299999997</v>
+        <v>39.881630000000001</v>
       </c>
       <c r="I154">
-        <v>-82.806872900000002</v>
+        <v>-83.094322000000005</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
@@ -5876,25 +5882,25 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>363</v>
+        <v>269</v>
       </c>
       <c r="C155" t="s">
         <v>125</v>
       </c>
       <c r="E155" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="F155" t="s">
-        <v>364</v>
+        <v>270</v>
       </c>
       <c r="G155" t="s">
         <v>328</v>
       </c>
       <c r="H155">
-        <v>39.760269000000001</v>
-      </c>
-      <c r="I155" s="2">
-        <v>-82.666267000000005</v>
+        <v>39.843274299999997</v>
+      </c>
+      <c r="I155">
+        <v>-82.806872900000002</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
@@ -5902,25 +5908,25 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C156" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E156" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="F156" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G156" t="s">
         <v>328</v>
       </c>
       <c r="H156">
-        <v>40.051938</v>
-      </c>
-      <c r="I156">
-        <v>-82.920542999999995</v>
+        <v>39.760269000000001</v>
+      </c>
+      <c r="I156" s="2">
+        <v>-82.666267000000005</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -5928,25 +5934,25 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C157" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="E157" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F157" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G157" t="s">
         <v>328</v>
       </c>
       <c r="H157">
-        <v>40.117525999999998</v>
-      </c>
-      <c r="I157" s="2">
-        <v>-82.986984000000007</v>
+        <v>40.051938</v>
+      </c>
+      <c r="I157">
+        <v>-82.920542999999995</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -5954,25 +5960,25 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C158" t="s">
         <v>30</v>
       </c>
       <c r="E158" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F158" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G158" t="s">
         <v>328</v>
       </c>
       <c r="H158">
-        <v>40.149245999999998</v>
-      </c>
-      <c r="I158">
-        <v>-83.091482999999997</v>
+        <v>40.117525999999998</v>
+      </c>
+      <c r="I158" s="2">
+        <v>-82.986984000000007</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -5980,28 +5986,25 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>145</v>
+        <v>369</v>
       </c>
       <c r="C159" t="s">
         <v>30</v>
       </c>
-      <c r="D159" t="s">
-        <v>371</v>
-      </c>
       <c r="E159" t="s">
         <v>11</v>
       </c>
       <c r="F159" t="s">
-        <v>146</v>
+        <v>370</v>
       </c>
       <c r="G159" t="s">
         <v>328</v>
       </c>
       <c r="H159">
-        <v>39.989275800000001</v>
+        <v>40.149245999999998</v>
       </c>
       <c r="I159">
-        <v>-83.052948999999998</v>
+        <v>-83.091482999999997</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -6009,25 +6012,28 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="C160" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="D160" t="s">
+        <v>371</v>
       </c>
       <c r="E160" t="s">
         <v>11</v>
       </c>
       <c r="F160" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="G160" t="s">
         <v>328</v>
       </c>
       <c r="H160">
-        <v>39.957871900000001</v>
+        <v>39.989275800000001</v>
       </c>
       <c r="I160">
-        <v>-83.011507600000002</v>
+        <v>-83.052948999999998</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
@@ -6035,7 +6041,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>372</v>
+        <v>174</v>
       </c>
       <c r="C161" t="s">
         <v>33</v>
@@ -6044,192 +6050,192 @@
         <v>11</v>
       </c>
       <c r="F161" t="s">
-        <v>231</v>
+        <v>175</v>
       </c>
       <c r="G161" t="s">
         <v>328</v>
       </c>
       <c r="H161">
-        <v>39.983791400000001</v>
+        <v>39.957871900000001</v>
       </c>
       <c r="I161">
-        <v>-83.0170332</v>
+        <v>-83.011507600000002</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C162" t="s">
-        <v>36</v>
-      </c>
-      <c r="D162" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E162" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F162" t="s">
-        <v>374</v>
+        <v>231</v>
       </c>
       <c r="G162" t="s">
         <v>328</v>
       </c>
       <c r="H162">
-        <v>39.994104200000002</v>
+        <v>39.983791400000001</v>
       </c>
       <c r="I162">
-        <v>-83.006157900000005</v>
+        <v>-83.0170332</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C163" t="s">
         <v>36</v>
       </c>
       <c r="D163" t="s">
-        <v>376</v>
+        <v>37</v>
       </c>
       <c r="E163" t="s">
         <v>41</v>
       </c>
       <c r="F163" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G163" t="s">
         <v>328</v>
       </c>
       <c r="H163">
-        <v>40.015101100000003</v>
+        <v>39.994104200000002</v>
       </c>
       <c r="I163">
-        <v>-83.011836200000005</v>
+        <v>-83.006157900000005</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C164" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D164" t="s">
-        <v>156</v>
+        <v>376</v>
       </c>
       <c r="E164" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="F164" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G164" t="s">
         <v>328</v>
       </c>
       <c r="H164">
-        <v>39.880431999999999</v>
+        <v>40.015101100000003</v>
       </c>
       <c r="I164">
-        <v>-83.070642000000007</v>
+        <v>-83.011836200000005</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>202</v>
+        <v>378</v>
       </c>
       <c r="C165" t="s">
-        <v>380</v>
+        <v>40</v>
+      </c>
+      <c r="D165" t="s">
+        <v>156</v>
       </c>
       <c r="E165" t="s">
         <v>11</v>
       </c>
       <c r="F165" t="s">
-        <v>203</v>
+        <v>379</v>
       </c>
       <c r="G165" t="s">
         <v>328</v>
       </c>
       <c r="H165">
-        <v>39.974749500000001</v>
+        <v>39.880431999999999</v>
       </c>
       <c r="I165">
-        <v>-83.026180499999995</v>
+        <v>-83.070642000000007</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>381</v>
+        <v>202</v>
       </c>
       <c r="C166" t="s">
-        <v>166</v>
-      </c>
-      <c r="D166" t="s">
-        <v>167</v>
+        <v>380</v>
       </c>
       <c r="E166" t="s">
         <v>11</v>
       </c>
       <c r="F166" t="s">
-        <v>382</v>
+        <v>203</v>
       </c>
       <c r="G166" t="s">
         <v>328</v>
       </c>
       <c r="H166">
-        <v>40.061892999999998</v>
+        <v>39.974749500000001</v>
       </c>
       <c r="I166">
-        <v>-83.075406999999998</v>
+        <v>-83.026180499999995</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
+        <v>165</v>
+      </c>
+      <c r="B167" t="s">
+        <v>381</v>
+      </c>
+      <c r="C167" t="s">
         <v>166</v>
       </c>
-      <c r="B167" t="s">
-        <v>39</v>
-      </c>
-      <c r="C167" t="s">
-        <v>44</v>
+      <c r="D167" t="s">
+        <v>167</v>
       </c>
       <c r="E167" t="s">
         <v>11</v>
       </c>
       <c r="F167" t="s">
-        <v>42</v>
+        <v>382</v>
       </c>
       <c r="G167" t="s">
         <v>328</v>
       </c>
       <c r="H167">
-        <v>39.944255400000003</v>
+        <v>40.061892999999998</v>
       </c>
       <c r="I167">
-        <v>-82.987217700000002</v>
+        <v>-83.075406999999998</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>383</v>
+        <v>39</v>
       </c>
       <c r="C168" t="s">
         <v>44</v>
@@ -6238,426 +6244,452 @@
         <v>11</v>
       </c>
       <c r="F168" t="s">
-        <v>384</v>
+        <v>42</v>
       </c>
       <c r="G168" t="s">
         <v>328</v>
       </c>
       <c r="H168">
-        <v>40.163572000000002</v>
+        <v>39.944255400000003</v>
       </c>
       <c r="I168">
-        <v>-83.074144000000004</v>
+        <v>-82.987217700000002</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C169" t="s">
-        <v>386</v>
+        <v>44</v>
       </c>
       <c r="E169" t="s">
         <v>11</v>
       </c>
       <c r="F169" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G169" t="s">
         <v>328</v>
       </c>
       <c r="H169">
-        <v>39.885311000000002</v>
+        <v>40.163572000000002</v>
       </c>
       <c r="I169">
-        <v>-82.754822000000004</v>
+        <v>-83.074144000000004</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C170" t="s">
-        <v>172</v>
+        <v>386</v>
       </c>
       <c r="E170" t="s">
         <v>11</v>
       </c>
       <c r="F170" t="s">
-        <v>81</v>
+        <v>387</v>
       </c>
       <c r="G170" t="s">
         <v>328</v>
       </c>
       <c r="H170">
-        <v>39.979754999999997</v>
+        <v>39.885311000000002</v>
       </c>
       <c r="I170">
-        <v>-83.033760000000001</v>
+        <v>-82.754822000000004</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C171" t="s">
         <v>172</v>
       </c>
       <c r="E171" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F171" t="s">
-        <v>390</v>
+        <v>81</v>
       </c>
       <c r="G171" t="s">
         <v>328</v>
       </c>
       <c r="H171">
-        <v>40.063040999999998</v>
+        <v>39.979754999999997</v>
       </c>
       <c r="I171">
-        <v>-83.056051600000004</v>
+        <v>-83.033760000000001</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C172" t="s">
-        <v>33</v>
+        <v>172</v>
       </c>
       <c r="E172" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F172" t="s">
-        <v>127</v>
+        <v>390</v>
       </c>
       <c r="G172" t="s">
-        <v>392</v>
+        <v>328</v>
       </c>
       <c r="H172">
-        <v>39.957180000000001</v>
+        <v>40.063040999999998</v>
       </c>
       <c r="I172">
-        <v>-83.012352000000007</v>
+        <v>-83.056051600000004</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C173" t="s">
-        <v>394</v>
-      </c>
-      <c r="D173" t="s">
-        <v>395</v>
+        <v>33</v>
       </c>
       <c r="E173" t="s">
         <v>11</v>
       </c>
       <c r="F173" t="s">
-        <v>396</v>
+        <v>127</v>
       </c>
       <c r="G173" t="s">
         <v>392</v>
       </c>
       <c r="H173">
-        <v>40.296548000000001</v>
+        <v>39.957180000000001</v>
       </c>
       <c r="I173">
-        <v>-83.449252000000001</v>
+        <v>-83.012352000000007</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C174" t="s">
-        <v>15</v>
+        <v>394</v>
       </c>
       <c r="D174" t="s">
-        <v>219</v>
+        <v>395</v>
       </c>
       <c r="E174" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="F174" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G174" t="s">
         <v>392</v>
       </c>
       <c r="H174">
-        <v>40.034066699999997</v>
+        <v>40.296548000000001</v>
       </c>
       <c r="I174">
-        <v>-83.016622999999996</v>
+        <v>-83.449252000000001</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C175" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D175" t="s">
-        <v>45</v>
+        <v>219</v>
       </c>
       <c r="E175" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="F175" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="G175" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="H175">
-        <v>40.298985999999999</v>
+        <v>40.034066699999997</v>
       </c>
       <c r="I175">
-        <v>-83.067916999999994</v>
+        <v>-83.016622999999996</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>309</v>
+        <v>399</v>
       </c>
       <c r="C176" t="s">
-        <v>166</v>
+        <v>44</v>
       </c>
       <c r="D176" t="s">
-        <v>167</v>
+        <v>45</v>
       </c>
       <c r="E176" t="s">
         <v>11</v>
       </c>
       <c r="F176" t="s">
-        <v>310</v>
+        <v>400</v>
       </c>
       <c r="G176" t="s">
         <v>401</v>
       </c>
       <c r="H176">
-        <v>40.020870000000002</v>
+        <v>40.298985999999999</v>
       </c>
       <c r="I176">
-        <v>-82.866675999999998</v>
+        <v>-83.067916999999994</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>263</v>
+        <v>309</v>
       </c>
       <c r="C177" t="s">
-        <v>125</v>
+        <v>166</v>
+      </c>
+      <c r="D177" t="s">
+        <v>167</v>
       </c>
       <c r="E177" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F177" t="s">
-        <v>264</v>
+        <v>310</v>
       </c>
       <c r="G177" t="s">
         <v>401</v>
       </c>
       <c r="H177">
-        <v>40.111477999999998</v>
+        <v>40.020870000000002</v>
       </c>
       <c r="I177">
-        <v>-82.945682000000005</v>
+        <v>-82.866675999999998</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>293</v>
+        <v>263</v>
       </c>
       <c r="C178" t="s">
-        <v>15</v>
-      </c>
-      <c r="D178" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="E178" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F178" t="s">
-        <v>294</v>
+        <v>264</v>
       </c>
       <c r="G178" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H178">
-        <v>39.986330100000004</v>
+        <v>40.111477999999998</v>
       </c>
       <c r="I178">
-        <v>-83.005578099999994</v>
+        <v>-82.945682000000005</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>403</v>
+        <v>293</v>
       </c>
       <c r="C179" t="s">
         <v>15</v>
       </c>
       <c r="D179" t="s">
-        <v>24</v>
+        <v>97</v>
       </c>
       <c r="E179" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="F179" t="s">
-        <v>404</v>
+        <v>294</v>
       </c>
       <c r="G179" t="s">
         <v>402</v>
       </c>
-      <c r="H179" s="3">
-        <v>40.000301</v>
+      <c r="H179">
+        <v>39.986330100000004</v>
       </c>
       <c r="I179">
-        <v>-82.998322000000002</v>
+        <v>-83.005578099999994</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C180" t="s">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="D180" t="s">
+        <v>24</v>
       </c>
       <c r="E180" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F180" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G180" t="s">
         <v>402</v>
       </c>
-      <c r="H180">
-        <v>40.063058099999999</v>
+      <c r="H180" s="3">
+        <v>40.000301</v>
       </c>
       <c r="I180">
-        <v>-83.017761100000001</v>
+        <v>-82.998322000000002</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C181" t="s">
-        <v>163</v>
+        <v>30</v>
       </c>
       <c r="E181" t="s">
-        <v>408</v>
+        <v>41</v>
       </c>
       <c r="F181" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="G181" t="s">
         <v>402</v>
       </c>
       <c r="H181">
-        <v>39.981107999999999</v>
+        <v>40.063058099999999</v>
       </c>
       <c r="I181">
-        <v>-82.998925</v>
+        <v>-83.017761100000001</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C182" t="s">
-        <v>411</v>
-      </c>
-      <c r="D182" t="s">
-        <v>411</v>
+        <v>163</v>
       </c>
       <c r="E182" t="s">
-        <v>17</v>
+        <v>408</v>
       </c>
       <c r="F182" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="G182" t="s">
         <v>402</v>
       </c>
       <c r="H182">
-        <v>40.022682000000003</v>
+        <v>39.981107999999999</v>
       </c>
       <c r="I182">
-        <v>-83.014105000000001</v>
+        <v>-82.998925</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>244</v>
+        <v>410</v>
       </c>
       <c r="C183" t="s">
-        <v>314</v>
+        <v>411</v>
+      </c>
+      <c r="D183" t="s">
+        <v>411</v>
       </c>
       <c r="E183" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F183" t="s">
-        <v>245</v>
+        <v>412</v>
       </c>
       <c r="G183" t="s">
         <v>402</v>
       </c>
       <c r="H183">
+        <v>40.022682000000003</v>
+      </c>
+      <c r="I183">
+        <v>-83.014105000000001</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A184" s="1">
+        <v>182</v>
+      </c>
+      <c r="B184" t="s">
+        <v>244</v>
+      </c>
+      <c r="C184" t="s">
+        <v>314</v>
+      </c>
+      <c r="E184" t="s">
+        <v>11</v>
+      </c>
+      <c r="F184" t="s">
+        <v>245</v>
+      </c>
+      <c r="G184" t="s">
+        <v>402</v>
+      </c>
+      <c r="H184">
         <v>39.963314199999999</v>
       </c>
-      <c r="I183">
+      <c r="I184">
         <v>-82.980843500000006</v>
       </c>
     </row>

</xml_diff>